<commit_message>
cierre 19 May 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/CREDITOS  ABASTOS  HERRADURA  ABRIL   2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/CREDITOS  ABASTOS  HERRADURA  ABRIL   2022.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15870" windowHeight="10305" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15870" windowHeight="10305" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES  ENERO  2022" sheetId="1" r:id="rId1"/>
     <sheet name="REMISIONES FEBRERO 2022" sheetId="2" r:id="rId2"/>
     <sheet name="REMISIONES   MARZO   2022  " sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="4" r:id="rId4"/>
+    <sheet name="REMISIONES   ABRIL  2022" sheetId="4" r:id="rId4"/>
     <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -686,6 +686,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -710,10 +714,6 @@
     <xf numFmtId="166" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1471,25 +1471,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="B2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -2237,12 +2237,12 @@
       <c r="B45" s="47"/>
       <c r="C45" s="48"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="70">
+      <c r="E45" s="72">
         <f>E41-G41</f>
         <v>0</v>
       </c>
-      <c r="F45" s="71"/>
-      <c r="G45" s="72"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="74"/>
       <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2258,11 +2258,11 @@
       <c r="B47" s="47"/>
       <c r="C47" s="48"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="73" t="s">
+      <c r="E47" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="F47" s="73"/>
-      <c r="G47" s="73"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="75"/>
       <c r="I47" s="2"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2404,25 +2404,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="B2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -3447,12 +3447,12 @@
       <c r="B55" s="47"/>
       <c r="C55" s="48"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="70">
+      <c r="E55" s="72">
         <f>E51-G51</f>
         <v>0</v>
       </c>
-      <c r="F55" s="71"/>
-      <c r="G55" s="72"/>
+      <c r="F55" s="73"/>
+      <c r="G55" s="74"/>
       <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3468,11 +3468,11 @@
       <c r="B57" s="47"/>
       <c r="C57" s="48"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="73" t="s">
+      <c r="E57" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="F57" s="73"/>
-      <c r="G57" s="73"/>
+      <c r="F57" s="75"/>
+      <c r="G57" s="75"/>
       <c r="I57" s="2"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3595,7 +3595,7 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:XFD1048576"/>
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3614,25 +3614,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="B2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -4579,12 +4579,12 @@
       <c r="B52" s="47"/>
       <c r="C52" s="48"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="70">
+      <c r="E52" s="72">
         <f>E48-G48</f>
         <v>0</v>
       </c>
-      <c r="F52" s="71"/>
-      <c r="G52" s="72"/>
+      <c r="F52" s="73"/>
+      <c r="G52" s="74"/>
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4600,11 +4600,11 @@
       <c r="B54" s="47"/>
       <c r="C54" s="48"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="73" t="s">
+      <c r="E54" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="F54" s="73"/>
-      <c r="G54" s="73"/>
+      <c r="F54" s="75"/>
+      <c r="G54" s="75"/>
       <c r="I54" s="2"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -4721,10 +4721,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4743,25 +4746,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="B2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -5689,8 +5692,8 @@
       <c r="E38" s="23">
         <v>11261</v>
       </c>
-      <c r="F38" s="74"/>
-      <c r="G38" s="75"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="67"/>
       <c r="H38" s="21">
         <f t="shared" si="0"/>
         <v>11261</v>
@@ -6412,12 +6415,12 @@
       <c r="B84" s="47"/>
       <c r="C84" s="48"/>
       <c r="D84" s="2"/>
-      <c r="E84" s="70">
+      <c r="E84" s="72">
         <f>E80-G80</f>
         <v>11261</v>
       </c>
-      <c r="F84" s="71"/>
-      <c r="G84" s="72"/>
+      <c r="F84" s="73"/>
+      <c r="G84" s="74"/>
       <c r="I84" s="2"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -6433,11 +6436,11 @@
       <c r="B86" s="47"/>
       <c r="C86" s="48"/>
       <c r="D86" s="2"/>
-      <c r="E86" s="73" t="s">
+      <c r="E86" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="F86" s="73"/>
-      <c r="G86" s="73"/>
+      <c r="F86" s="75"/>
+      <c r="G86" s="75"/>
       <c r="I86" s="2"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>